<commit_message>
last commit for assignment 2
</commit_message>
<xml_diff>
--- a/Assignment_2/documentation/report.xlsx
+++ b/Assignment_2/documentation/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repo\.vscode\Parallal_algorithm\Assignment_2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFBDDCF-2124-4485-A6DD-F285EA941B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9631FB31-8E4B-418F-AA05-42453EC15B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01FC82E5-F3B0-42A5-8B07-DA479F104F21}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>n</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>MPI-based TSP (nanosecond)</t>
+  </si>
+  <si>
+    <t>N (Number of Block x Block Size)</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Execution Time among Serial, Threaded, and Mpi-based TSP</a:t>
+              <a:t> Execution Time for Serial TSP</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -552,6 +555,1106 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A864-4578-9595-8B54557EFF54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1298941936"/>
+        <c:axId val="1298949008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1298941936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Number of Cities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298949008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1298949008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Execution Time (in Nano Second)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.1251758087201125E-2"/>
+              <c:y val="0.27188211887845098"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298941936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Execution Time for Threaded TSP</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threaded TSP (nanosecond)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$41:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$41:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1030834200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1080946800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1041580600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1611682100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2353034800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8362454400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66091837600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CC2-4044-A027-916F09F61CA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1298941936"/>
+        <c:axId val="1298949008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1298941936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Number of Cities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298949008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1298949008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Execution Time (in Nano Second)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.1251758087201125E-2"/>
+              <c:y val="0.27188211887845098"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298941936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Execution Time for MPI-based TSP</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$75</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI-based TSP (nanosecond)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$76:$C$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$76:$D$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1008484500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1005727800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1048154200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1391129300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2467518200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13380199600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87808032500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-69A8-4D27-AC95-049C7398EFFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -915,7 +2018,1129 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1469,6 +3694,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>4764</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A86C522-6493-475A-8FA6-DEFFD7CF7C30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>14289</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAB31003-049B-417C-BF72-6ADEA275FB66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1774,10 +4075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76EB544-A70A-42DD-9136-8DC9A82342BC}">
-  <dimension ref="B4:E12"/>
+  <dimension ref="B4:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="T70" sqref="T70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,6 +4186,136 @@
       </c>
       <c r="E12" s="4"/>
     </row>
+    <row r="39" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="3">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1030834200</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="3">
+        <v>100</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1080946800</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1041580600</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1611682100</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D45" s="4">
+        <v>2353034800</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8362454400</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D47" s="4">
+        <v>66091837600</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="3:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="3">
+        <v>10</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1008484500</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="3">
+        <v>100</v>
+      </c>
+      <c r="D77" s="4">
+        <v>1005727800</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D78" s="4">
+        <v>1048154200</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1391129300</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D80" s="4">
+        <v>2467518200</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D81" s="4">
+        <v>13380199600</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="D82" s="4">
+        <v>87808032500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>